<commit_message>
Updated device inventory servicessssaa
</commit_message>
<xml_diff>
--- a/FAST_BACKEND/device_report.xlsx
+++ b/FAST_BACKEND/device_report.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W48"/>
+  <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,14 +470,14 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Stack</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>PSU Count</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Stack</t>
-        </is>
-      </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
           <t>PSU Model</t>
@@ -550,30 +550,30 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>SW Vulnerability Support EoS</t>
+          <t>SW Vulnerability Support EoSError Message</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>R_167_SW_02</t>
+          <t>R_384</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ExtremeXOS</t>
+          <t>HuaweiOS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>X450a-24tdc</t>
+          <t>S5335-L24T4X-D1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10.200.97.71</t>
+          <t>169.254.2.2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -582,26 +582,34 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>715</v>
+      </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>333</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>82.43000000000001</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>39.47</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
@@ -614,7 +622,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>R_167_SW_01</t>
+          <t>R_167_SW_02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -630,7 +638,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10.200.97.72</t>
+          <t>10.200.97.71</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -639,26 +647,34 @@
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>715</v>
+      </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>341</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>383</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>89.03</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>56.28</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
@@ -671,27 +687,23 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SULY-EAPC-CI-COM-003</t>
+          <t>R_383</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>apic</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>FCH2052V2HM</t>
-        </is>
-      </c>
+          <t>HuaweiOS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>APIC-SERVER-L2</t>
+          <t>S5335-L24T4X-D1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>172.8.0.3</t>
+          <t>169.254.2.1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -700,17 +712,25 @@
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>715</v>
+      </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>343</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>407</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>84.28</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -719,54 +739,36 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2" t="n">
-        <v>43545</v>
-      </c>
-      <c r="R4" s="2" t="n">
-        <v>45708</v>
-      </c>
-      <c r="S4" s="2" t="n">
-        <v>45473</v>
-      </c>
-      <c r="T4" s="2" t="n">
-        <v>44001</v>
-      </c>
-      <c r="U4" s="2" t="n">
-        <v>45184</v>
-      </c>
-      <c r="V4" s="2" t="n">
-        <v>44366</v>
-      </c>
-      <c r="W4" s="2" t="n">
-        <v>44731</v>
-      </c>
+        <v>0.14</v>
+      </c>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-402</t>
+          <t>R_167_SW_01</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>apic</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>FDO205209PH</t>
-        </is>
-      </c>
+          <t>ExtremeXOS</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>N9K-C93180YC-EX</t>
+          <t>X450a-24tdc</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>172.8.144.79</t>
+          <t>10.200.97.72</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -775,53 +777,47 @@
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>715</v>
+      </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>383</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>87.73</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>81.38</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2" t="n">
-        <v>45793</v>
-      </c>
-      <c r="R5" s="2" t="n">
-        <v>45788</v>
-      </c>
-      <c r="S5" s="2" t="n">
-        <v>46630</v>
-      </c>
-      <c r="T5" s="2" t="n">
-        <v>45793</v>
-      </c>
-      <c r="U5" s="2" t="n">
-        <v>45794</v>
-      </c>
-      <c r="V5" s="2" t="n">
-        <v>45785</v>
-      </c>
-      <c r="W5" s="2" t="n">
-        <v>45792</v>
-      </c>
+        <v>0.14</v>
+      </c>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-431</t>
+          <t>SULY-EAPC-CI-COM-003</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -831,17 +827,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>FDO204813YQ</t>
+          <t>FCH2052V2HM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>APIC-SERVER-L2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>172.8.16.77</t>
+          <t>172.8.0.3</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -850,45 +846,59 @@
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>715</v>
+      </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>337</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>382</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>88.22</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>178.22</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q6" s="2" t="n">
-        <v>44417</v>
+        <v>43545</v>
       </c>
       <c r="R6" s="2" t="n">
-        <v>44782</v>
+        <v>45708</v>
       </c>
       <c r="S6" s="2" t="n">
-        <v>46630</v>
-      </c>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
+        <v>45473</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>44001</v>
+      </c>
+      <c r="U6" s="2" t="n">
+        <v>45184</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <v>44366</v>
+      </c>
       <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-314</t>
+          <t>SULY-ELEF-CI-COM-402</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -898,17 +908,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>FDO21142F3D</t>
+          <t>FDO205209PH</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>N9K-C93180YC-EX</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>172.8.144.91</t>
+          <t>172.8.144.79</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -917,45 +927,59 @@
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>715</v>
+      </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>388</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>86.59999999999999</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>84.81</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q7" s="2" t="n">
-        <v>44417</v>
+        <v>45793</v>
       </c>
       <c r="R7" s="2" t="n">
-        <v>44782</v>
+        <v>45788</v>
       </c>
       <c r="S7" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
+      <c r="T7" s="2" t="n">
+        <v>45793</v>
+      </c>
+      <c r="U7" s="2" t="n">
+        <v>45794</v>
+      </c>
+      <c r="V7" s="2" t="n">
+        <v>45785</v>
+      </c>
       <c r="W7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-426</t>
+          <t>SULY-ELEF-CI-COM-431</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -965,17 +989,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>FDO21150F8Z</t>
+          <t>FDO204813YQ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>N9K-C93180YC-EX</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>172.8.144.71</t>
+          <t>172.8.16.77</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -984,53 +1008,53 @@
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>715</v>
+      </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>352</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>90.26000000000001</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>120.18</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q8" s="2" t="n">
-        <v>45793</v>
+        <v>44417</v>
       </c>
       <c r="R8" s="2" t="n">
-        <v>45788</v>
+        <v>44782</v>
       </c>
       <c r="S8" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T8" s="2" t="n">
-        <v>45793</v>
-      </c>
-      <c r="U8" s="2" t="n">
-        <v>45794</v>
-      </c>
-      <c r="V8" s="2" t="n">
-        <v>45785</v>
-      </c>
-      <c r="W8" s="2" t="n">
-        <v>45792</v>
-      </c>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-309</t>
+          <t>SULY-ELEF-CI-COM-314</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1040,7 +1064,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>FDO21142F2K</t>
+          <t>FDO21142F3D</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1050,7 +1074,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>172.8.16.69</t>
+          <t>172.8.144.91</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1059,26 +1083,34 @@
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>715</v>
+      </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>345</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>368</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>93.75</v>
       </c>
       <c r="N9" t="n">
         <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>170.45</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q9" s="2" t="n">
         <v>44417</v>
@@ -1097,7 +1129,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-311</t>
+          <t>SULY-ELEF-CI-COM-426</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1107,17 +1139,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>FDO21141MXL</t>
+          <t>FDO21150F8Z</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>N9K-C93180YC-EX</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>172.8.16.70</t>
+          <t>172.8.144.71</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1126,45 +1158,59 @@
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>715</v>
+      </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>335</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>382</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>87.7</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>149.44</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q10" s="2" t="n">
-        <v>44417</v>
+        <v>45793</v>
       </c>
       <c r="R10" s="2" t="n">
-        <v>44782</v>
+        <v>45788</v>
       </c>
       <c r="S10" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
+      <c r="T10" s="2" t="n">
+        <v>45793</v>
+      </c>
+      <c r="U10" s="2" t="n">
+        <v>45794</v>
+      </c>
+      <c r="V10" s="2" t="n">
+        <v>45785</v>
+      </c>
       <c r="W10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-429</t>
+          <t>SULY-ELEF-CI-COM-309</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1174,7 +1220,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FDO204813ZF</t>
+          <t>FDO21142F2K</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1184,7 +1230,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>172.8.16.66</t>
+          <t>172.8.16.69</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1193,26 +1239,34 @@
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>715</v>
+      </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>332</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>396</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>83.84</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>75.28</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="Q11" s="2" t="n">
         <v>44417</v>
@@ -1231,7 +1285,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-307</t>
+          <t>SULY-ELEF-CI-COM-311</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1241,7 +1295,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>FDO21140B30</t>
+          <t>FDO21141MXL</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1251,7 +1305,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>172.8.16.67</t>
+          <t>172.8.16.70</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1260,26 +1314,34 @@
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>715</v>
+      </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>405</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>86.42</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>66.59</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q12" s="2" t="n">
         <v>44417</v>
@@ -1298,7 +1360,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-423</t>
+          <t>SULY-ELEF-CI-COM-429</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1308,7 +1370,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>FDO21142F55</t>
+          <t>FDO204813ZF</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1318,35 +1380,43 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>172.8.144.75</t>
+          <t>172.8.16.66</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Jebal Ali</t>
+          <t>SULAY</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>715</v>
+      </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>382</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>88.48</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>57.68</v>
+        <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q13" s="2" t="n">
         <v>44417</v>
@@ -1365,7 +1435,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-447</t>
+          <t>SULY-ELEF-CI-COM-307</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1375,54 +1445,62 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>FDO264407ZZ</t>
+          <t>FDO21140B30</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>N9K-C93360YC-FX2</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>172.8.16.80</t>
+          <t>172.8.16.67</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Jebal Ali</t>
+          <t>SULAY</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>715</v>
+      </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>379</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>86.81</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>102.53</v>
+        <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="Q14" s="2" t="n">
-        <v>43718</v>
+        <v>44417</v>
       </c>
       <c r="R14" s="2" t="n">
-        <v>44083</v>
+        <v>44782</v>
       </c>
       <c r="S14" s="2" t="n">
-        <v>45930</v>
+        <v>46630</v>
       </c>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
@@ -1432,27 +1510,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>SULY-ESPN-CI-COM-104</t>
+          <t>SULY-ELEF-CI-COM-423</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>apic</t>
+          <t>cisco_nxos</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>FOX2049GGYK</t>
+          <t>FDO21142F55</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>N9K-C9504</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>172.8.144.68</t>
+          <t>172.8.144.75</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1461,17 +1539,25 @@
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>715</v>
+      </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>342</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>85.93000000000001</v>
       </c>
       <c r="N15" t="n">
         <v>0</v>
@@ -1480,11 +1566,17 @@
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
+        <v>0.14</v>
+      </c>
+      <c r="Q15" s="2" t="n">
+        <v>44417</v>
+      </c>
+      <c r="R15" s="2" t="n">
+        <v>44782</v>
+      </c>
+      <c r="S15" s="2" t="n">
+        <v>46630</v>
+      </c>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
@@ -1493,7 +1585,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-418</t>
+          <t>SULY-ELEF-CI-COM-447</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1503,17 +1595,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>FDO21140JUT</t>
+          <t>FDO264407ZZ</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>N9K-C93360YC-FX2</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>172.8.144.88</t>
+          <t>172.8.16.80</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1522,35 +1614,43 @@
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>715</v>
+      </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>89.47</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>160.06</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q16" s="2" t="n">
-        <v>44417</v>
+        <v>43718</v>
       </c>
       <c r="R16" s="2" t="n">
-        <v>44782</v>
+        <v>44083</v>
       </c>
       <c r="S16" s="2" t="n">
-        <v>46630</v>
+        <v>45930</v>
       </c>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
@@ -1560,7 +1660,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-301</t>
+          <t>SULY-ESPN-CI-COM-104</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1570,17 +1670,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>FDO20531JSF</t>
+          <t>FOX2049GGYK</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>N9K-C93180YC-EX</t>
+          <t>N9K-C9504</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>172.8.160.69</t>
+          <t>172.8.144.68</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1589,73 +1689,67 @@
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>715</v>
+      </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>344</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>392</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>87.76000000000001</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>59.45</v>
+        <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="2" t="n">
-        <v>45793</v>
-      </c>
-      <c r="R17" s="2" t="n">
-        <v>45788</v>
-      </c>
-      <c r="S17" s="2" t="n">
-        <v>46630</v>
-      </c>
-      <c r="T17" s="2" t="n">
-        <v>45793</v>
-      </c>
-      <c r="U17" s="2" t="n">
-        <v>45794</v>
-      </c>
-      <c r="V17" s="2" t="n">
-        <v>45785</v>
-      </c>
-      <c r="W17" s="2" t="n">
-        <v>45792</v>
-      </c>
+        <v>0.14</v>
+      </c>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SULY-EAPC-CI-COM-002</t>
+          <t>SULY-ELEF-CI-COM-418</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>cisco_ios</t>
+          <t>apic</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>FCH2052V2FU</t>
+          <t>FDO21140JUT</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>APIC-SERVER-L2</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>172.8.0.2</t>
+          <t>172.8.144.88</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1664,17 +1758,25 @@
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>715</v>
+      </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>326</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>383</v>
       </c>
       <c r="M18" t="n">
-        <v>0</v>
+        <v>85.12</v>
       </c>
       <c r="N18" t="n">
         <v>0</v>
@@ -1683,34 +1785,26 @@
         <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="Q18" s="2" t="n">
-        <v>43545</v>
+        <v>44417</v>
       </c>
       <c r="R18" s="2" t="n">
-        <v>45708</v>
+        <v>44782</v>
       </c>
       <c r="S18" s="2" t="n">
-        <v>45473</v>
-      </c>
-      <c r="T18" s="2" t="n">
-        <v>44001</v>
-      </c>
-      <c r="U18" s="2" t="n">
-        <v>45184</v>
-      </c>
-      <c r="V18" s="2" t="n">
-        <v>44366</v>
-      </c>
-      <c r="W18" s="2" t="n">
-        <v>44731</v>
-      </c>
+        <v>46630</v>
+      </c>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-432</t>
+          <t>SULY-ELEF-CI-COM-301</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1720,131 +1814,159 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>FDO21190NND</t>
+          <t>FDO20531JSF</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>N9K-C93180YC-EX</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>172.8.160.75</t>
+          <t>172.8.160.69</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>SULAY</t>
+          <t>Jebal Ali</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>715</v>
+      </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>392</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>86.48</v>
       </c>
       <c r="N19" t="n">
         <v>0</v>
       </c>
       <c r="O19" t="n">
-        <v>164.4</v>
+        <v>0</v>
       </c>
       <c r="P19" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q19" s="2" t="n">
-        <v>44417</v>
+        <v>45793</v>
       </c>
       <c r="R19" s="2" t="n">
-        <v>44782</v>
+        <v>45788</v>
       </c>
       <c r="S19" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr"/>
+      <c r="T19" s="2" t="n">
+        <v>45793</v>
+      </c>
+      <c r="U19" s="2" t="n">
+        <v>45794</v>
+      </c>
+      <c r="V19" s="2" t="n">
+        <v>45785</v>
+      </c>
       <c r="W19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-315</t>
+          <t>SULY-EAPC-CI-COM-002</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>apic</t>
+          <t>cisco_ios</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>FDO21190NLC</t>
+          <t>FCH2052V2FU</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>APIC-SERVER-L2</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>172.8.160.76</t>
+          <t>10.64.252.68</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>SULAY</t>
+          <t>Jebal Ali</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>715</v>
+      </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>355</v>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
+        <v>94.67</v>
       </c>
       <c r="N20" t="n">
         <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>142.46</v>
+        <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q20" s="2" t="n">
-        <v>44417</v>
+        <v>43545</v>
       </c>
       <c r="R20" s="2" t="n">
-        <v>44782</v>
+        <v>45708</v>
       </c>
       <c r="S20" s="2" t="n">
-        <v>46630</v>
-      </c>
-      <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
-      <c r="V20" t="inlineStr"/>
+        <v>45473</v>
+      </c>
+      <c r="T20" s="2" t="n">
+        <v>44001</v>
+      </c>
+      <c r="U20" s="2" t="n">
+        <v>45184</v>
+      </c>
+      <c r="V20" s="2" t="n">
+        <v>44366</v>
+      </c>
       <c r="W20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-403</t>
+          <t>SULY-ELEF-CI-COM-432</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1854,7 +1976,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>FDO204813ZE</t>
+          <t>FDO21190NND</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1864,7 +1986,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>172.8.144.77</t>
+          <t>172.8.160.75</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1873,26 +1995,34 @@
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>715</v>
+      </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>342</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>383</v>
       </c>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>89.3</v>
       </c>
       <c r="N21" t="n">
         <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>46.87</v>
+        <v>0</v>
       </c>
       <c r="P21" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q21" s="2" t="n">
         <v>44417</v>
@@ -1911,7 +2041,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-304</t>
+          <t>SULY-ELEF-CI-COM-315</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1921,7 +2051,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>FDO2043157K</t>
+          <t>FDO21190NLC</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1931,7 +2061,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>172.8.144.81</t>
+          <t>172.8.160.76</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1940,26 +2070,34 @@
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>715</v>
+      </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>345</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>87.79000000000001</v>
       </c>
       <c r="N22" t="n">
         <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>169.18</v>
+        <v>0</v>
       </c>
       <c r="P22" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q22" s="2" t="n">
         <v>44417</v>
@@ -1978,27 +2116,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-415</t>
+          <t>SULY-ELEF-CI-COM-403</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>cisco_ios</t>
+          <t>apic</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>FDO21153153</t>
+          <t>FDO204813ZE</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>N9K-C93180YC-EX</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>172.8.160.70</t>
+          <t>172.8.144.77</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2007,53 +2145,53 @@
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>715</v>
+      </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>88.05</v>
       </c>
       <c r="N23" t="n">
         <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="P23" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q23" s="2" t="n">
-        <v>45793</v>
+        <v>44417</v>
       </c>
       <c r="R23" s="2" t="n">
-        <v>45788</v>
+        <v>44782</v>
       </c>
       <c r="S23" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T23" s="2" t="n">
-        <v>45793</v>
-      </c>
-      <c r="U23" s="2" t="n">
-        <v>45794</v>
-      </c>
-      <c r="V23" s="2" t="n">
-        <v>45785</v>
-      </c>
-      <c r="W23" s="2" t="n">
-        <v>45792</v>
-      </c>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SULY-ESPN-CI-COM-102</t>
+          <t>SULY-ELEF-CI-COM-304</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2063,36 +2201,44 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>FOX2049GGYF</t>
+          <t>FDO2043157K</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>N9K-C9504</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>172.8.144.67</t>
+          <t>172.8.144.81</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Jebal Ali</t>
+          <t>SULAY</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>715</v>
+      </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>387</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>85.01000000000001</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
@@ -2101,11 +2247,17 @@
         <v>0</v>
       </c>
       <c r="P24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr"/>
-      <c r="S24" t="inlineStr"/>
+        <v>0.13</v>
+      </c>
+      <c r="Q24" s="2" t="n">
+        <v>44417</v>
+      </c>
+      <c r="R24" s="2" t="n">
+        <v>44782</v>
+      </c>
+      <c r="S24" s="2" t="n">
+        <v>46630</v>
+      </c>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
@@ -2114,82 +2266,88 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-444</t>
+          <t>SULY-ELEF-CI-COM-415</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>apic</t>
+          <t>cisco_ios</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>FDO25300JFD</t>
+          <t>FDO21153153</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-FX</t>
+          <t>N9K-C93180YC-EX</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>172.8.160.68</t>
+          <t>172.8.160.70</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Jebal Ali</t>
+          <t>SULAY</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>715</v>
+      </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>328</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>381</v>
       </c>
       <c r="M25" t="n">
-        <v>0</v>
+        <v>86.09</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>64.16</v>
+        <v>0</v>
       </c>
       <c r="P25" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="Q25" s="2" t="n">
-        <v>45139</v>
+        <v>45793</v>
       </c>
       <c r="R25" s="2" t="n">
-        <v>45703</v>
+        <v>45788</v>
       </c>
       <c r="S25" s="2" t="n">
-        <v>47330</v>
+        <v>46630</v>
       </c>
       <c r="T25" s="2" t="n">
-        <v>45869</v>
+        <v>45793</v>
       </c>
       <c r="U25" s="2" t="n">
-        <v>47055</v>
+        <v>45794</v>
       </c>
       <c r="V25" s="2" t="n">
-        <v>46599</v>
-      </c>
-      <c r="W25" s="2" t="n">
-        <v>47330</v>
-      </c>
+        <v>45785</v>
+      </c>
+      <c r="W25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-303</t>
+          <t>SULY-ESPN-CI-COM-102</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2199,17 +2357,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>FDO20460EKD</t>
+          <t>FOX2049GGYF</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>N9K-C9504</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>172.8.144.69</t>
+          <t>172.8.144.67</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2218,17 +2376,25 @@
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
+        <v>715</v>
+      </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>346</v>
       </c>
       <c r="L26" t="n">
-        <v>0</v>
+        <v>371</v>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>93.26000000000001</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
@@ -2237,17 +2403,11 @@
         <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="2" t="n">
-        <v>44417</v>
-      </c>
-      <c r="R26" s="2" t="n">
-        <v>44782</v>
-      </c>
-      <c r="S26" s="2" t="n">
-        <v>46630</v>
-      </c>
+        <v>0.14</v>
+      </c>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr"/>
@@ -2256,7 +2416,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-420</t>
+          <t>SULY-ELEF-CI-COM-303</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2266,7 +2426,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>FDO21141MUY</t>
+          <t>FDO20460EKD</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2276,7 +2436,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>172.8.160.73</t>
+          <t>172.8.144.69</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2285,26 +2445,34 @@
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>715</v>
+      </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="L27" t="n">
-        <v>0</v>
+        <v>371</v>
       </c>
       <c r="M27" t="n">
-        <v>0</v>
+        <v>90.56999999999999</v>
       </c>
       <c r="N27" t="n">
         <v>0</v>
       </c>
       <c r="O27" t="n">
-        <v>141</v>
+        <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q27" s="2" t="n">
         <v>44417</v>
@@ -2323,7 +2491,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-430</t>
+          <t>SULY-ELEF-CI-COM-420</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2333,7 +2501,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>FDO211325Q9</t>
+          <t>FDO21141MUY</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2343,7 +2511,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>172.8.144.86</t>
+          <t>172.8.160.73</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2352,26 +2520,34 @@
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>715</v>
+      </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>343</v>
       </c>
       <c r="L28" t="n">
-        <v>0</v>
+        <v>378</v>
       </c>
       <c r="M28" t="n">
-        <v>0</v>
+        <v>90.73999999999999</v>
       </c>
       <c r="N28" t="n">
         <v>0</v>
       </c>
       <c r="O28" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="P28" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q28" s="2" t="n">
         <v>44417</v>
@@ -2390,7 +2566,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-312</t>
+          <t>SULY-ELEF-CI-COM-430</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2400,7 +2576,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>FDO211311DA</t>
+          <t>FDO211325Q9</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2410,7 +2586,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>172.8.16.72</t>
+          <t>172.8.144.86</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2419,26 +2595,34 @@
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>715</v>
+      </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>341</v>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
+        <v>397</v>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>85.89</v>
       </c>
       <c r="N29" t="n">
         <v>0</v>
       </c>
       <c r="O29" t="n">
-        <v>84.65000000000001</v>
+        <v>0</v>
       </c>
       <c r="P29" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q29" s="2" t="n">
         <v>44417</v>
@@ -2457,7 +2641,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-412</t>
+          <t>SULY-ELEF-CI-COM-312</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2467,7 +2651,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>FDO21142F5G</t>
+          <t>FDO211311DA</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2477,7 +2661,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>172.8.16.74</t>
+          <t>172.8.16.72</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2486,26 +2670,34 @@
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>715</v>
+      </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>344</v>
       </c>
       <c r="L30" t="n">
-        <v>0</v>
+        <v>386</v>
       </c>
       <c r="M30" t="n">
-        <v>0</v>
+        <v>89.12</v>
       </c>
       <c r="N30" t="n">
         <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>142.95</v>
+        <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q30" s="2" t="n">
         <v>44417</v>
@@ -2524,7 +2716,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-446</t>
+          <t>SULY-ELEF-CI-COM-412</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2534,17 +2726,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>FDO264407XL</t>
+          <t>FDO21142F5G</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>N9K-C93360YC-FX2</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>172.8.144.80</t>
+          <t>172.8.16.74</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2553,35 +2745,43 @@
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
+      <c r="H31" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>715</v>
+      </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="M31" t="n">
-        <v>0</v>
+        <v>89.20999999999999</v>
       </c>
       <c r="N31" t="n">
         <v>0</v>
       </c>
       <c r="O31" t="n">
-        <v>111.82</v>
+        <v>0</v>
       </c>
       <c r="P31" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q31" s="2" t="n">
-        <v>43718</v>
+        <v>44417</v>
       </c>
       <c r="R31" s="2" t="n">
-        <v>44083</v>
+        <v>44782</v>
       </c>
       <c r="S31" s="2" t="n">
-        <v>45930</v>
+        <v>46630</v>
       </c>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
@@ -2591,7 +2791,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-417</t>
+          <t>SULY-ELEF-CI-COM-446</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2601,17 +2801,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>FDO21140JXA</t>
+          <t>FDO264407XL</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>N9K-C93360YC-FX2</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>172.8.160.71</t>
+          <t>172.8.144.80</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2620,35 +2820,43 @@
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
+        <v>715</v>
+      </c>
       <c r="K32" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="L32" t="n">
-        <v>0</v>
+        <v>379</v>
       </c>
       <c r="M32" t="n">
-        <v>0</v>
+        <v>89.70999999999999</v>
       </c>
       <c r="N32" t="n">
         <v>0</v>
       </c>
       <c r="O32" t="n">
-        <v>184.91</v>
+        <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q32" s="2" t="n">
-        <v>44417</v>
+        <v>43718</v>
       </c>
       <c r="R32" s="2" t="n">
-        <v>44782</v>
+        <v>44083</v>
       </c>
       <c r="S32" s="2" t="n">
-        <v>46630</v>
+        <v>45930</v>
       </c>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
@@ -2658,7 +2866,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-308</t>
+          <t>SULY-ELEF-CI-COM-417</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2668,7 +2876,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>FDO21142F0S</t>
+          <t>FDO21140JXA</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2678,7 +2886,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>172.8.16.68</t>
+          <t>172.8.160.71</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2687,26 +2895,34 @@
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
+        <v>715</v>
+      </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>326</v>
       </c>
       <c r="L33" t="n">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="M33" t="n">
-        <v>0</v>
+        <v>82.95</v>
       </c>
       <c r="N33" t="n">
         <v>0</v>
       </c>
       <c r="O33" t="n">
-        <v>114.39</v>
+        <v>0</v>
       </c>
       <c r="P33" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="Q33" s="2" t="n">
         <v>44417</v>
@@ -2725,7 +2941,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-424</t>
+          <t>SULY-ELEF-CI-COM-308</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2735,7 +2951,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>FDO21142F2V</t>
+          <t>FDO21142F0S</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2745,35 +2961,43 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>172.8.160.74</t>
+          <t>172.8.16.68</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Duha</t>
+          <t>Jebal Ali</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
+        <v>715</v>
+      </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>354</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>381</v>
       </c>
       <c r="M34" t="n">
-        <v>0</v>
+        <v>92.91</v>
       </c>
       <c r="N34" t="n">
         <v>0</v>
       </c>
       <c r="O34" t="n">
-        <v>41.7</v>
+        <v>0</v>
       </c>
       <c r="P34" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q34" s="2" t="n">
         <v>44417</v>
@@ -2792,7 +3016,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-427</t>
+          <t>SULY-ELEF-CI-COM-424</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2802,72 +3026,72 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>FDO21160ZYT</t>
+          <t>FDO21142F2V</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>N9K-C93180YC-EX</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>172.8.144.73</t>
+          <t>172.8.160.74</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Jebal Ali</t>
+          <t>Duha</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
+      <c r="H35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
+        <v>715</v>
+      </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>352</v>
       </c>
       <c r="L35" t="n">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="M35" t="n">
-        <v>0</v>
+        <v>93.87</v>
       </c>
       <c r="N35" t="n">
         <v>0</v>
       </c>
       <c r="O35" t="n">
-        <v>181.73</v>
+        <v>0</v>
       </c>
       <c r="P35" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q35" s="2" t="n">
-        <v>45793</v>
+        <v>44417</v>
       </c>
       <c r="R35" s="2" t="n">
-        <v>45788</v>
+        <v>44782</v>
       </c>
       <c r="S35" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T35" s="2" t="n">
-        <v>45793</v>
-      </c>
-      <c r="U35" s="2" t="n">
-        <v>45794</v>
-      </c>
-      <c r="V35" s="2" t="n">
-        <v>45785</v>
-      </c>
-      <c r="W35" s="2" t="n">
-        <v>45792</v>
-      </c>
+      <c r="T35" t="inlineStr"/>
+      <c r="U35" t="inlineStr"/>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>SULY-ESLR-CI-COM-201</t>
+          <t>SULY-ELEF-CI-COM-427</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2877,7 +3101,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>FDO21160ZVE</t>
+          <t>FDO21160ZYT</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2887,7 +3111,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>172.8.144.72</t>
+          <t>172.8.144.73</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2896,26 +3120,34 @@
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J36" t="n">
+        <v>715</v>
+      </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>343</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>386</v>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>88.86</v>
       </c>
       <c r="N36" t="n">
         <v>0</v>
       </c>
       <c r="O36" t="n">
-        <v>76.14</v>
+        <v>0</v>
       </c>
       <c r="P36" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q36" s="2" t="n">
         <v>45793</v>
@@ -2935,14 +3167,12 @@
       <c r="V36" s="2" t="n">
         <v>45785</v>
       </c>
-      <c r="W36" s="2" t="n">
-        <v>45792</v>
-      </c>
+      <c r="W36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-409</t>
+          <t>SULY-ESLR-CI-COM-201</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2952,7 +3182,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>FDO211531A3</t>
+          <t>FDO21160ZVE</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2962,7 +3192,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>172.8.160.64</t>
+          <t>172.8.144.72</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2971,26 +3201,34 @@
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
+      <c r="H37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
+        <v>715</v>
+      </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>392</v>
       </c>
       <c r="M37" t="n">
-        <v>0</v>
+        <v>89.29000000000001</v>
       </c>
       <c r="N37" t="n">
         <v>0</v>
       </c>
       <c r="O37" t="n">
-        <v>174.07</v>
+        <v>0</v>
       </c>
       <c r="P37" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q37" s="2" t="n">
         <v>45793</v>
@@ -3010,14 +3248,12 @@
       <c r="V37" s="2" t="n">
         <v>45785</v>
       </c>
-      <c r="W37" s="2" t="n">
-        <v>45792</v>
-      </c>
+      <c r="W37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-438</t>
+          <t>SULY-ELEF-CI-COM-409</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3027,17 +3263,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>FDO20481405</t>
+          <t>FDO211531A3</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>N9K-C93180YC-EX</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>172.8.16.87</t>
+          <t>172.8.160.64</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3046,45 +3282,59 @@
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J38" t="n">
+        <v>715</v>
+      </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>352</v>
       </c>
       <c r="L38" t="n">
-        <v>0</v>
+        <v>382</v>
       </c>
       <c r="M38" t="n">
-        <v>0</v>
+        <v>92.15000000000001</v>
       </c>
       <c r="N38" t="n">
         <v>0</v>
       </c>
       <c r="O38" t="n">
-        <v>102.47</v>
+        <v>0</v>
       </c>
       <c r="P38" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q38" s="2" t="n">
-        <v>44417</v>
+        <v>45793</v>
       </c>
       <c r="R38" s="2" t="n">
-        <v>44782</v>
+        <v>45788</v>
       </c>
       <c r="S38" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
-      <c r="V38" t="inlineStr"/>
+      <c r="T38" s="2" t="n">
+        <v>45793</v>
+      </c>
+      <c r="U38" s="2" t="n">
+        <v>45794</v>
+      </c>
+      <c r="V38" s="2" t="n">
+        <v>45785</v>
+      </c>
       <c r="W38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-443</t>
+          <t>SULY-ELEF-CI-COM-438</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3094,7 +3344,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>FDO21140JVX</t>
+          <t>FDO20481405</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3104,7 +3354,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>172.8.16.88</t>
+          <t>172.8.16.87</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3113,26 +3363,34 @@
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr"/>
+      <c r="H39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J39" t="n">
+        <v>715</v>
+      </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="L39" t="n">
-        <v>0</v>
+        <v>383</v>
       </c>
       <c r="M39" t="n">
-        <v>0</v>
+        <v>88.25</v>
       </c>
       <c r="N39" t="n">
         <v>0</v>
       </c>
       <c r="O39" t="n">
-        <v>90.42</v>
+        <v>0</v>
       </c>
       <c r="P39" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q39" s="2" t="n">
         <v>44417</v>
@@ -3151,7 +3409,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>SULY-ESPN-CI-COM-101</t>
+          <t>SULY-ELEF-CI-COM-443</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3161,17 +3419,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>FOX2049G2YX</t>
+          <t>FDO21140JVX</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>N9K-C9504</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>172.8.144.65</t>
+          <t>172.8.16.88</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3180,17 +3438,25 @@
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
+      <c r="H40" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J40" t="n">
+        <v>715</v>
+      </c>
       <c r="K40" t="n">
-        <v>0</v>
+        <v>341</v>
       </c>
       <c r="L40" t="n">
-        <v>0</v>
+        <v>386</v>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>88.34</v>
       </c>
       <c r="N40" t="n">
         <v>0</v>
@@ -3199,11 +3465,17 @@
         <v>0</v>
       </c>
       <c r="P40" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr"/>
-      <c r="S40" t="inlineStr"/>
+        <v>0.14</v>
+      </c>
+      <c r="Q40" s="2" t="n">
+        <v>44417</v>
+      </c>
+      <c r="R40" s="2" t="n">
+        <v>44782</v>
+      </c>
+      <c r="S40" s="2" t="n">
+        <v>46630</v>
+      </c>
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="inlineStr"/>
@@ -3212,7 +3484,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-411</t>
+          <t>SULY-ESPN-CI-COM-101</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3222,17 +3494,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>FDO21142F5K</t>
+          <t>FOX2049G2YX</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>N9K-C9504</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>172.8.16.73</t>
+          <t>172.8.144.65</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3241,36 +3513,38 @@
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
+      <c r="H41" t="n">
+        <v>1</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J41" t="n">
+        <v>715</v>
+      </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>354</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="M41" t="n">
-        <v>0</v>
+        <v>94.40000000000001</v>
       </c>
       <c r="N41" t="n">
         <v>0</v>
       </c>
       <c r="O41" t="n">
-        <v>150.87</v>
+        <v>0</v>
       </c>
       <c r="P41" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="2" t="n">
-        <v>44417</v>
-      </c>
-      <c r="R41" s="2" t="n">
-        <v>44782</v>
-      </c>
-      <c r="S41" s="2" t="n">
-        <v>46630</v>
-      </c>
+        <v>0.14</v>
+      </c>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
       <c r="V41" t="inlineStr"/>
@@ -3279,7 +3553,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-319</t>
+          <t>SULY-ELEF-CI-COM-411</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3289,72 +3563,72 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>FDO21162J2G</t>
+          <t>FDO21142F5K</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>N9K-C93180YC-EX</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>172.8.16.65</t>
+          <t>172.8.16.73</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Duha</t>
+          <t>Jebal Ali</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr"/>
+      <c r="H42" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J42" t="n">
+        <v>715</v>
+      </c>
       <c r="K42" t="n">
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>379</v>
       </c>
       <c r="M42" t="n">
-        <v>0</v>
+        <v>89.45</v>
       </c>
       <c r="N42" t="n">
         <v>0</v>
       </c>
       <c r="O42" t="n">
-        <v>169.35</v>
+        <v>0</v>
       </c>
       <c r="P42" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q42" s="2" t="n">
-        <v>45793</v>
+        <v>44417</v>
       </c>
       <c r="R42" s="2" t="n">
-        <v>45788</v>
+        <v>44782</v>
       </c>
       <c r="S42" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T42" s="2" t="n">
-        <v>45793</v>
-      </c>
-      <c r="U42" s="2" t="n">
-        <v>45794</v>
-      </c>
-      <c r="V42" s="2" t="n">
-        <v>45785</v>
-      </c>
-      <c r="W42" s="2" t="n">
-        <v>45792</v>
-      </c>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-305</t>
+          <t>SULY-ELEF-CI-COM-319</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3364,17 +3638,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>FDO21140JYA</t>
+          <t>FDO21162J2G</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>N9K-C93180YC-EX</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>172.8.160.72</t>
+          <t>172.8.16.65</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3383,65 +3657,79 @@
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
+      <c r="H43" t="n">
+        <v>1</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J43" t="n">
+        <v>715</v>
+      </c>
       <c r="K43" t="n">
-        <v>0</v>
+        <v>342</v>
       </c>
       <c r="L43" t="n">
-        <v>0</v>
+        <v>388</v>
       </c>
       <c r="M43" t="n">
-        <v>0</v>
+        <v>88.14</v>
       </c>
       <c r="N43" t="n">
         <v>0</v>
       </c>
       <c r="O43" t="n">
-        <v>161.99</v>
+        <v>0</v>
       </c>
       <c r="P43" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q43" s="2" t="n">
-        <v>44417</v>
+        <v>45793</v>
       </c>
       <c r="R43" s="2" t="n">
-        <v>44782</v>
+        <v>45788</v>
       </c>
       <c r="S43" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
-      <c r="V43" t="inlineStr"/>
+      <c r="T43" s="2" t="n">
+        <v>45793</v>
+      </c>
+      <c r="U43" s="2" t="n">
+        <v>45794</v>
+      </c>
+      <c r="V43" s="2" t="n">
+        <v>45785</v>
+      </c>
       <c r="W43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-448</t>
+          <t>SULY-ELEF-CI-COM-305</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>cisco_nxos</t>
+          <t>apic</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>FDO26250DWB</t>
+          <t>FDO21140JYA</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>N9K-C9336C-FX2</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>172.8.144.78</t>
+          <t>172.8.160.72</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3450,35 +3738,43 @@
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr"/>
+      <c r="H44" t="n">
+        <v>1</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J44" t="n">
+        <v>715</v>
+      </c>
       <c r="K44" t="n">
-        <v>0</v>
+        <v>342</v>
       </c>
       <c r="L44" t="n">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="M44" t="n">
-        <v>0</v>
+        <v>84.65000000000001</v>
       </c>
       <c r="N44" t="n">
         <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>183.51</v>
+        <v>0</v>
       </c>
       <c r="P44" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q44" s="2" t="n">
-        <v>44252</v>
+        <v>44417</v>
       </c>
       <c r="R44" s="2" t="n">
-        <v>44617</v>
+        <v>44782</v>
       </c>
       <c r="S44" s="2" t="n">
-        <v>46446</v>
+        <v>46630</v>
       </c>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr"/>
@@ -3488,7 +3784,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-302</t>
+          <t>SULY-ELEF-CI-COM-448</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3498,17 +3794,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>FDO2053179K</t>
+          <t>FDO26250DWB</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>N9K-C93180YC-EX</t>
+          <t>N9K-C9336C-FX2</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>172.8.144.83</t>
+          <t>172.8.144.78</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3517,53 +3813,53 @@
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J45" t="n">
+        <v>715</v>
+      </c>
       <c r="K45" t="n">
-        <v>0</v>
+        <v>353</v>
       </c>
       <c r="L45" t="n">
-        <v>0</v>
+        <v>372</v>
       </c>
       <c r="M45" t="n">
-        <v>0</v>
+        <v>94.89</v>
       </c>
       <c r="N45" t="n">
         <v>0</v>
       </c>
       <c r="O45" t="n">
-        <v>176.25</v>
+        <v>0</v>
       </c>
       <c r="P45" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q45" s="2" t="n">
-        <v>45793</v>
+        <v>44252</v>
       </c>
       <c r="R45" s="2" t="n">
-        <v>45788</v>
+        <v>44617</v>
       </c>
       <c r="S45" s="2" t="n">
-        <v>46630</v>
-      </c>
-      <c r="T45" s="2" t="n">
-        <v>45793</v>
-      </c>
-      <c r="U45" s="2" t="n">
-        <v>45794</v>
-      </c>
-      <c r="V45" s="2" t="n">
-        <v>45785</v>
-      </c>
-      <c r="W45" s="2" t="n">
-        <v>45792</v>
-      </c>
+        <v>46446</v>
+      </c>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-419</t>
+          <t>SULY-ELEF-CI-COM-302</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3573,17 +3869,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>FDO211325NQ</t>
+          <t>FDO2053179K</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>N9K-C93180YC-EX</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>172.8.144.74</t>
+          <t>172.8.144.83</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3592,120 +3888,134 @@
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
+      <c r="H46" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J46" t="n">
+        <v>715</v>
+      </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>356</v>
       </c>
       <c r="L46" t="n">
-        <v>0</v>
+        <v>382</v>
       </c>
       <c r="M46" t="n">
-        <v>0</v>
+        <v>93.19</v>
       </c>
       <c r="N46" t="n">
         <v>0</v>
       </c>
       <c r="O46" t="n">
-        <v>91.34999999999999</v>
+        <v>0</v>
       </c>
       <c r="P46" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q46" s="2" t="n">
-        <v>44417</v>
+        <v>45793</v>
       </c>
       <c r="R46" s="2" t="n">
-        <v>44782</v>
+        <v>45788</v>
       </c>
       <c r="S46" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
-      <c r="V46" t="inlineStr"/>
+      <c r="T46" s="2" t="n">
+        <v>45793</v>
+      </c>
+      <c r="U46" s="2" t="n">
+        <v>45794</v>
+      </c>
+      <c r="V46" s="2" t="n">
+        <v>45785</v>
+      </c>
       <c r="W46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-405</t>
+          <t>SULY-ELEF-CI-COM-419</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>apic</t>
+          <t>cisco_nxos</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>FDO2052228W</t>
+          <t>FDO211325NQ</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>N9K-C93180YC-EX</t>
+          <t>N9K-C93108TC-EX</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>172.8.144.82</t>
+          <t>172.8.144.74</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Jebal Ali</t>
+          <t>Duha</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr"/>
-      <c r="J47" t="inlineStr"/>
+      <c r="H47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J47" t="n">
+        <v>715</v>
+      </c>
       <c r="K47" t="n">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="L47" t="n">
-        <v>0</v>
+        <v>386</v>
       </c>
       <c r="M47" t="n">
-        <v>0</v>
+        <v>90.16</v>
       </c>
       <c r="N47" t="n">
         <v>0</v>
       </c>
       <c r="O47" t="n">
-        <v>152.41</v>
+        <v>0</v>
       </c>
       <c r="P47" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="Q47" s="2" t="n">
-        <v>45793</v>
+        <v>44417</v>
       </c>
       <c r="R47" s="2" t="n">
-        <v>45788</v>
+        <v>44782</v>
       </c>
       <c r="S47" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T47" s="2" t="n">
-        <v>45793</v>
-      </c>
-      <c r="U47" s="2" t="n">
-        <v>45794</v>
-      </c>
-      <c r="V47" s="2" t="n">
-        <v>45785</v>
-      </c>
-      <c r="W47" s="2" t="n">
-        <v>45792</v>
-      </c>
+      <c r="T47" t="inlineStr"/>
+      <c r="U47" t="inlineStr"/>
+      <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>SULY-ELEF-CI-COM-318</t>
+          <t>SULY-ELEF-CI-COM-405</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3715,17 +4025,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>FDO21132JU9</t>
+          <t>FDO2052228W</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>N9K-C93108TC-EX</t>
+          <t>N9K-C93180YC-EX</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>172.8.16.75</t>
+          <t>172.8.144.82</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -3734,40 +4044,129 @@
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
-      <c r="J48" t="inlineStr"/>
+      <c r="H48" t="n">
+        <v>1</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J48" t="n">
+        <v>715</v>
+      </c>
       <c r="K48" t="n">
-        <v>0</v>
+        <v>333</v>
       </c>
       <c r="L48" t="n">
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="M48" t="n">
-        <v>0</v>
+        <v>83.67</v>
       </c>
       <c r="N48" t="n">
         <v>0</v>
       </c>
       <c r="O48" t="n">
-        <v>97.66</v>
+        <v>0</v>
       </c>
       <c r="P48" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="Q48" s="2" t="n">
-        <v>44417</v>
+        <v>45793</v>
       </c>
       <c r="R48" s="2" t="n">
-        <v>44782</v>
+        <v>45788</v>
       </c>
       <c r="S48" s="2" t="n">
         <v>46630</v>
       </c>
-      <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr"/>
-      <c r="V48" t="inlineStr"/>
+      <c r="T48" s="2" t="n">
+        <v>45793</v>
+      </c>
+      <c r="U48" s="2" t="n">
+        <v>45794</v>
+      </c>
+      <c r="V48" s="2" t="n">
+        <v>45785</v>
+      </c>
       <c r="W48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>SULY-ELEF-CI-COM-318</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>apic</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>FDO21132JU9</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>N9K-C93108TC-EX</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>172.8.16.75</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Jebal Ali</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>pkw-sdldf-715k</t>
+        </is>
+      </c>
+      <c r="J49" t="n">
+        <v>715</v>
+      </c>
+      <c r="K49" t="n">
+        <v>330</v>
+      </c>
+      <c r="L49" t="n">
+        <v>374</v>
+      </c>
+      <c r="M49" t="n">
+        <v>88.23999999999999</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="Q49" s="2" t="n">
+        <v>44417</v>
+      </c>
+      <c r="R49" s="2" t="n">
+        <v>44782</v>
+      </c>
+      <c r="S49" s="2" t="n">
+        <v>46630</v>
+      </c>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="inlineStr"/>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>